<commit_message>
Removed console logging | Added summary.txt
</commit_message>
<xml_diff>
--- a/1111417799_3695883753/src/data-points.xlsx
+++ b/1111417799_3695883753/src/data-points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruch0401/Desktop/USC/CSCI-570 AOA/CSCI570-FinalProject/1111417799_3695883753/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D37AC4B-85A6-6045-B49F-9104468233AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6916AA4B-2D67-874F-AF77-9881F88E89C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1A4E9A9B-0B7A-AF47-AFB8-4C98532C2522}"/>
   </bookViews>
@@ -421,7 +421,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -483,13 +483,13 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2374,6 +2374,1349 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time Comparison (Basic + Efficient)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (Basic Version)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.5664E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3722000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7712999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8745999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6012000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1336999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0671000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.102338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.7193999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C4A-6244-A1BC-84691C3FE190}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (Efficient Version)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.6088999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2650999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0409999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4169999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.276E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4367999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.101427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15668699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.108246</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4C4A-6244-A1BC-84691C3FE190}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="891410064"/>
+        <c:axId val="891411712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="891410064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Problem Size (Sum of Input Strings)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="891411712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="891411712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> (In seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="891410064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory Comparison (Basic + Efficient)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$D$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Memory (Basic Version)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$C$26:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$D$26:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>554.9609375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>554.9765625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1026.046875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2050.046875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2129.890625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7249.890625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14338.109375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31559.796875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-00A6-564B-9A1E-D574CA1F376C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$E$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Memory (Efficient Version)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$C$26:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$E$26:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>554.9609375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1026.03125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2050.03125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3626.9609375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4098.109375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14338.109375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4393.9296875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23340.0546875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-00A6-564B-9A1E-D574CA1F376C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1393275504"/>
+        <c:axId val="1393277152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1393275504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Problem Size (Sum of the Input</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> Strings)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1393277152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1393277152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> Required (in KBs)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1393275504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2414,7 +3757,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2971,15 +5426,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2999,6 +5454,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C20B705-CB08-7340-A522-EBC4BD1FDB02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28E573D-B139-8048-9DB1-3A07CE08F950}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3306,8 +5835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A248488D-C59D-3F48-A86D-7DC726E2FF52}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>